<commit_message>
Da debuggare: 1. colori markers nella mappa 2. righe dello stesso colore in tabella 3. caratteri spuri dovuti all' Unicode
</commit_message>
<xml_diff>
--- a/view_portate/static/data/Misuratori installati.xlsx
+++ b/view_portate/static/data/Misuratori installati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Geronazzo\PycharmProjects\sceintificProject\test_PortalePortate\view_portate\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefano Trevisan\PycharmProjects\PortaleHydroTest23\view_portate\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8B0ECF-21FE-4E27-BCF4-A787CB248CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFCD858-974B-45FD-8430-42B59E9E9556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12168" xr2:uid="{A8FBCE24-CB40-49BB-A0BA-A74F57FC9EE6}"/>
+    <workbookView xWindow="-28920" yWindow="1695" windowWidth="29040" windowHeight="15720" xr2:uid="{A8FBCE24-CB40-49BB-A0BA-A74F57FC9EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Marca</t>
   </si>
@@ -71,24 +71,6 @@
     <t>MTTHSL-1</t>
   </si>
   <si>
-    <t>Camera di manovra - "Acquedotto Merone"</t>
-  </si>
-  <si>
-    <t>Pozzetto SA3 - Condotta di adduzione alla turbina</t>
-  </si>
-  <si>
-    <t>Fine concessione</t>
-  </si>
-  <si>
-    <t>Pozzetto SA3 - Condotta principale DN1600</t>
-  </si>
-  <si>
-    <t>MTTHSL (vecchio modello)</t>
-  </si>
-  <si>
-    <t>ND</t>
-  </si>
-  <si>
     <t>Centrale CU4</t>
   </si>
   <si>
@@ -107,9 +89,6 @@
     <t>Da definire</t>
   </si>
   <si>
-    <t>III salto "Acquedotto Merone"</t>
-  </si>
-  <si>
     <t>101FUDTL-1NA</t>
   </si>
   <si>
@@ -123,15 +102,85 @@
   </si>
   <si>
     <t>areatecnica</t>
+  </si>
+  <si>
+    <t>Stato</t>
+  </si>
+  <si>
+    <t>In servizio</t>
+  </si>
+  <si>
+    <t>II salto Acquedotto Merone</t>
+  </si>
+  <si>
+    <t>III salto Acquedotto Merone</t>
+  </si>
+  <si>
+    <t>I salto Acquedotto Merone (camera di manovra)</t>
+  </si>
+  <si>
+    <t>Scarico DN800 SA3</t>
+  </si>
+  <si>
+    <t>Da rilevare</t>
+  </si>
+  <si>
+    <t>Non noto</t>
+  </si>
+  <si>
+    <t>Da installare</t>
+  </si>
+  <si>
+    <t>Vasca di carico SA6</t>
+  </si>
+  <si>
+    <t>FU0112301358</t>
+  </si>
+  <si>
+    <t>2 misuratori non funzionanti</t>
+  </si>
+  <si>
+    <t>Da prendere</t>
+  </si>
+  <si>
+    <t>Guasto</t>
+  </si>
+  <si>
+    <t>Acquedotto Zumpo</t>
+  </si>
+  <si>
+    <t>In valutazione</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Sorical Differenzi Partitore Musco 2</t>
+  </si>
+  <si>
+    <t>Sorical Pisarello</t>
+  </si>
+  <si>
+    <t>Portata media globale</t>
+  </si>
+  <si>
+    <t>Dev portata</t>
+  </si>
+  <si>
+    <t>Ultimo timestamp</t>
+  </si>
+  <si>
+    <t>Ultimo valore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -168,11 +217,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -191,9 +242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -231,7 +282,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -337,7 +388,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -479,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -487,26 +538,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0A6A60-2D40-4A33-9311-7DC98C003A7E}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -523,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -535,10 +592,25 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -557,7 +629,7 @@
       <c r="F2" s="2">
         <v>39.860159540162002</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>16.508604884147601</v>
       </c>
       <c r="H2" s="1">
@@ -566,10 +638,25 @@
       <c r="I2" s="1">
         <v>45412</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2">
+        <v>56.7</v>
+      </c>
+      <c r="M2">
+        <v>21.8</v>
+      </c>
+      <c r="N2" s="5">
+        <v>45267.49496527778</v>
+      </c>
+      <c r="O2">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -586,7 +673,7 @@
       <c r="F3" s="3">
         <v>39.176653030236999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>16.341715157031999</v>
       </c>
       <c r="H3" s="1">
@@ -595,136 +682,293 @@
       <c r="I3" s="1">
         <v>45350</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>160</v>
+      </c>
+      <c r="M3">
+        <v>13</v>
+      </c>
+      <c r="N3" s="5">
+        <v>45212.796875</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>21835595</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45301</v>
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F4" s="3">
-        <v>38.966011694532398</v>
-      </c>
-      <c r="G4">
-        <v>17.081366479396799</v>
-      </c>
-      <c r="H4" s="1">
-        <v>45169</v>
-      </c>
-      <c r="I4" t="s">
+        <v>38.966487179835198</v>
+      </c>
+      <c r="G4" s="4">
+        <v>17.081208229064899</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="J4" t="s">
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3">
+        <v>38.947994000000001</v>
+      </c>
+      <c r="G5" s="4">
+        <v>17.01379</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44861</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45224</v>
+      </c>
+      <c r="F6" s="3">
+        <v>39.281429509517999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>16.261447370052299</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45224</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6">
+        <v>112</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6" s="1">
+        <v>45265.496527777781</v>
+      </c>
+      <c r="O6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45231</v>
+      </c>
+      <c r="F7" s="2">
+        <v>38.943868897832203</v>
+      </c>
+      <c r="G7" s="4">
+        <v>17.052621245384199</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45275</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45.753760728503103</v>
+      </c>
+      <c r="G8" s="4">
+        <v>11.7688493353564</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1">
-        <v>45301</v>
-      </c>
-      <c r="F5" s="3">
-        <v>38.966487179835198</v>
-      </c>
-      <c r="G5">
-        <v>17.081208229064899</v>
-      </c>
-      <c r="H5" s="1">
-        <v>44215</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F9" s="3">
+        <v>39.1856847281285</v>
+      </c>
+      <c r="G9" s="4">
+        <v>16.330734193325</v>
+      </c>
+      <c r="J9" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3">
-        <v>38.947994000000001</v>
-      </c>
-      <c r="G6">
-        <v>17.01379</v>
-      </c>
-      <c r="H6" s="1">
-        <v>44861</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1">
-        <v>45224</v>
-      </c>
-      <c r="F7" s="3">
-        <v>39.281429509517999</v>
-      </c>
-      <c r="G7">
-        <v>16.261447370052299</v>
-      </c>
-      <c r="H7" s="1">
-        <v>45224</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45.763760728503101</v>
+      </c>
+      <c r="G10" s="4">
+        <v>11.7788493353564</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="2">
+        <v>45.763760728503101</v>
+      </c>
+      <c r="G11" s="4">
+        <v>11.7688493353564</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2">
+        <v>45.763760728503101</v>
+      </c>
+      <c r="G12" s="4">
+        <v>11.7588493353564</v>
+      </c>
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="2">
+        <v>45.773760728503099</v>
+      </c>
+      <c r="G13" s="4">
+        <v>11.7688493353564</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sistemate le posizioni dei misuratori Inseriti misuratori in valutazione
</commit_message>
<xml_diff>
--- a/view_portate/static/data/Misuratori installati.xlsx
+++ b/view_portate/static/data/Misuratori installati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Geronazzo\PycharmProjects\Portale_Hydro\view_portate\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefano Trevisan\PycharmProjects\PortaleHydro\view_portate\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3040F5B-1BFC-4398-96D5-401F94BCCE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E1BA3A-253E-4380-9D93-031AE92512A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8FBCE24-CB40-49BB-A0BA-A74F57FC9EE6}"/>
+    <workbookView xWindow="-28920" yWindow="1695" windowWidth="29040" windowHeight="15720" xr2:uid="{A8FBCE24-CB40-49BB-A0BA-A74F57FC9EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>Marca</t>
   </si>
@@ -104,9 +104,6 @@
     <t>III salto Acquedotto Merone</t>
   </si>
   <si>
-    <t>I salto Acquedotto Merone (camera di manovra)</t>
-  </si>
-  <si>
     <t>Scarico DN800 SA3</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>SA</t>
   </si>
   <si>
-    <t>Sorical Differenzi Partitore Musco 2</t>
-  </si>
-  <si>
-    <t>Sorical Pisarello</t>
-  </si>
-  <si>
     <t>Punto_di_misura</t>
   </si>
   <si>
@@ -171,6 +162,21 @@
   </si>
   <si>
     <t>Ultimo_timestamp</t>
+  </si>
+  <si>
+    <t>Camera di manovra Merone</t>
+  </si>
+  <si>
+    <t>Sorgente Zumpo</t>
+  </si>
+  <si>
+    <t>Sorical Differenzi Murate / Pisarello</t>
+  </si>
+  <si>
+    <t>Inacessibile</t>
+  </si>
+  <si>
+    <t>I salto Acquedotto Merone</t>
   </si>
 </sst>
 </file>
@@ -241,9 +247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +287,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -387,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0A6A60-2D40-4A33-9311-7DC98C003A7E}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +561,7 @@
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -564,7 +570,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -576,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -585,10 +591,10 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -597,16 +603,16 @@
         <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -626,10 +632,10 @@
         <v>45301</v>
       </c>
       <c r="F2" s="2">
-        <v>39.860159540162002</v>
+        <v>39.860277777777782</v>
       </c>
       <c r="G2" s="4">
-        <v>16.508604884147601</v>
+        <v>16.508611111111112</v>
       </c>
       <c r="H2" s="1">
         <v>45141</v>
@@ -655,7 +661,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -670,10 +676,10 @@
         <v>45301</v>
       </c>
       <c r="F3" s="3">
-        <v>39.176653030236999</v>
+        <v>39.176666666666669</v>
       </c>
       <c r="G3" s="4">
-        <v>16.341715157031999</v>
+        <v>16.341666666666665</v>
       </c>
       <c r="H3" s="1">
         <v>45162</v>
@@ -699,7 +705,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -708,10 +714,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="3">
         <v>38.966487179835198</v>
@@ -724,7 +730,7 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -813,7 +819,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -822,7 +828,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
         <v>45231</v>
@@ -849,7 +855,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -858,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -873,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N8" s="1"/>
     </row>
@@ -888,7 +894,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3">
         <v>39.1856847281285</v>
@@ -900,83 +906,102 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2">
-        <v>45.763760728503101</v>
+        <v>39.240833333333335</v>
       </c>
       <c r="G10" s="4">
-        <v>11.7788493353564</v>
+        <v>16.361944444444447</v>
       </c>
       <c r="J10" t="s">
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2">
-        <v>45.763760728503101</v>
+        <v>39.231111111111112</v>
       </c>
       <c r="G11" s="4">
-        <v>11.7688493353564</v>
+        <v>16.404999999999998</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2">
-        <v>45.763760728503101</v>
+        <v>38.999938888888892</v>
       </c>
       <c r="G12" s="4">
-        <v>11.7588493353564</v>
+        <v>17.062283333333333</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F13" s="2">
-        <v>45.773760728503099</v>
+        <v>39.116572222222224</v>
       </c>
       <c r="G13" s="4">
-        <v>11.7688493353564</v>
+        <v>16.749461111111113</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="23" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <f>39+10/60+55/3600</f>
+        <v>39.18194444444444</v>
+      </c>
+      <c r="G14">
+        <f>16+20/60+9/3600</f>
+        <v>16.335833333333333</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Merge tra versioni Stefano e David
</commit_message>
<xml_diff>
--- a/view_portate/static/data/Misuratori installati.xlsx
+++ b/view_portate/static/data/Misuratori installati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Geronazzo\PycharmProjects\Portale_Hydro\view_portate\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefano Trevisan\PycharmProjects\PortaleHydro\view_portate\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3040F5B-1BFC-4398-96D5-401F94BCCE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E1BA3A-253E-4380-9D93-031AE92512A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8FBCE24-CB40-49BB-A0BA-A74F57FC9EE6}"/>
+    <workbookView xWindow="-28920" yWindow="1695" windowWidth="29040" windowHeight="15720" xr2:uid="{A8FBCE24-CB40-49BB-A0BA-A74F57FC9EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>Marca</t>
   </si>
@@ -104,9 +104,6 @@
     <t>III salto Acquedotto Merone</t>
   </si>
   <si>
-    <t>I salto Acquedotto Merone (camera di manovra)</t>
-  </si>
-  <si>
     <t>Scarico DN800 SA3</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>SA</t>
   </si>
   <si>
-    <t>Sorical Differenzi Partitore Musco 2</t>
-  </si>
-  <si>
-    <t>Sorical Pisarello</t>
-  </si>
-  <si>
     <t>Punto_di_misura</t>
   </si>
   <si>
@@ -171,6 +162,21 @@
   </si>
   <si>
     <t>Ultimo_timestamp</t>
+  </si>
+  <si>
+    <t>Camera di manovra Merone</t>
+  </si>
+  <si>
+    <t>Sorgente Zumpo</t>
+  </si>
+  <si>
+    <t>Sorical Differenzi Murate / Pisarello</t>
+  </si>
+  <si>
+    <t>Inacessibile</t>
+  </si>
+  <si>
+    <t>I salto Acquedotto Merone</t>
   </si>
 </sst>
 </file>
@@ -241,9 +247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +287,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -387,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0A6A60-2D40-4A33-9311-7DC98C003A7E}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +561,7 @@
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -564,7 +570,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -576,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -585,10 +591,10 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -597,16 +603,16 @@
         <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -626,10 +632,10 @@
         <v>45301</v>
       </c>
       <c r="F2" s="2">
-        <v>39.860159540162002</v>
+        <v>39.860277777777782</v>
       </c>
       <c r="G2" s="4">
-        <v>16.508604884147601</v>
+        <v>16.508611111111112</v>
       </c>
       <c r="H2" s="1">
         <v>45141</v>
@@ -655,7 +661,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -670,10 +676,10 @@
         <v>45301</v>
       </c>
       <c r="F3" s="3">
-        <v>39.176653030236999</v>
+        <v>39.176666666666669</v>
       </c>
       <c r="G3" s="4">
-        <v>16.341715157031999</v>
+        <v>16.341666666666665</v>
       </c>
       <c r="H3" s="1">
         <v>45162</v>
@@ -699,7 +705,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -708,10 +714,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F4" s="3">
         <v>38.966487179835198</v>
@@ -724,7 +730,7 @@
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1"/>
     </row>
@@ -813,7 +819,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -822,7 +828,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
         <v>45231</v>
@@ -849,7 +855,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -858,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -873,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N8" s="1"/>
     </row>
@@ -888,7 +894,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3">
         <v>39.1856847281285</v>
@@ -900,83 +906,102 @@
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2">
-        <v>45.763760728503101</v>
+        <v>39.240833333333335</v>
       </c>
       <c r="G10" s="4">
-        <v>11.7788493353564</v>
+        <v>16.361944444444447</v>
       </c>
       <c r="J10" t="s">
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2">
-        <v>45.763760728503101</v>
+        <v>39.231111111111112</v>
       </c>
       <c r="G11" s="4">
-        <v>11.7688493353564</v>
+        <v>16.404999999999998</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2">
-        <v>45.763760728503101</v>
+        <v>38.999938888888892</v>
       </c>
       <c r="G12" s="4">
-        <v>11.7588493353564</v>
+        <v>17.062283333333333</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F13" s="2">
-        <v>45.773760728503099</v>
+        <v>39.116572222222224</v>
       </c>
       <c r="G13" s="4">
-        <v>11.7688493353564</v>
+        <v>16.749461111111113</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="23" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14">
+        <f>39+10/60+55/3600</f>
+        <v>39.18194444444444</v>
+      </c>
+      <c r="G14">
+        <f>16+20/60+9/3600</f>
+        <v>16.335833333333333</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>